<commit_message>
template changes for circulator
</commit_message>
<xml_diff>
--- a/controllers/Attachment 1 - Circulator ER Template.xlsx
+++ b/controllers/Attachment 1 - Circulator ER Template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\33 ENERGY RATING PROGRAM\Circulator Pump\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sfrees/projects/hi-er/controllers/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4167E983-C5AB-1C4B-9596-13169F591C62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="34020" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Import-Export Sheet" sheetId="1" r:id="rId1"/>
@@ -355,32 +356,146 @@
     <t>Most Consumptive Pressure Curve</t>
   </si>
   <si>
-    <r>
-      <t>Input the Rated (Least Consumptive) control method used on the pump.
-No speed control
+    <t>External Input Signal Only Control</t>
+  </si>
+  <si>
+    <t>External Input Signal and Other Controls</t>
+  </si>
+  <si>
+    <t>Manual Speed Controls</t>
+  </si>
+  <si>
+    <t>CP1: Wet Rotor
+CP2: Dry Rotor Two Piece
+CP3: Dry Rotor Three Piece</t>
+  </si>
+  <si>
+    <t>Control Methods</t>
+  </si>
+  <si>
+    <t>Rated (Least consumptive) HI Energy Rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Least consumptive) load point weigted average input power at maximum rotating speed </t>
+  </si>
+  <si>
+    <t>Rated (Least consumptive) load point weighted average input power at reduced speeds</t>
+  </si>
+  <si>
+    <t>If Pressure speed control is the rated (least consumptive) control method, insert the control curve equation as function of flow rate(x) and head (y). For example y=mx+b or y=ax^2+bx+c, etc.</t>
+  </si>
+  <si>
+    <t>If Pressure speed control is the most consumptive control method, insert the control curve equation as function of flow rate(x) and head(y). For example y=mx+b or y=ax^2+bx+c, etc.</t>
+  </si>
+  <si>
+    <t>Participant/Manufacturer</t>
+  </si>
+  <si>
+    <t>Rated (Least consumptive) Weighted Average Input Power</t>
+  </si>
+  <si>
+    <t>Pressure  Control</t>
+  </si>
+  <si>
+    <t>Tempertature  Control</t>
+  </si>
+  <si>
+    <t>I. No Speed Control</t>
+  </si>
+  <si>
+    <t>II. Pressure  Control</t>
+  </si>
+  <si>
+    <t>III. Temperature Control</t>
+  </si>
+  <si>
+    <t>IV. External Input Signal only  Control</t>
+  </si>
+  <si>
+    <t>VI. Manual Speed Control</t>
+  </si>
+  <si>
+    <t>Input values of maximum and reduced weighted average input power for only control methods V and VI.</t>
+  </si>
+  <si>
+    <t>Input control input power values for only control methods I, II, III, and IV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Method II.
+Select Yes if pump uses pressure speed control</t>
+  </si>
+  <si>
+    <t>Method III.
+Select Yes if pump uses temperature speed control</t>
+  </si>
+  <si>
+    <t>Method IV.
+Select Yes if pump uses external input only speed control</t>
+  </si>
+  <si>
+    <t>Method V.
+Select Yes if pump uses external input speed control and other controls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method VI.
+Select Yes if pump uses manual speed control </t>
+  </si>
+  <si>
+    <t>Fill in for all control methods if applicable</t>
+  </si>
+  <si>
+    <t>Input control input power values for only control methods I, II, III, and IV. Fill in if applicable.</t>
+  </si>
+  <si>
+    <t>Input values of maximum and reduced weighted average input power for only control methods V and VI. Fill in if applicable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Least consumptive) load point driver or control input power  at 25% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Least consumptive) load point driver or control input power at 50% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Least consumptive) load point driver or control  input power at 75% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rated (Least consumptive) load point driver or control input power at 100% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most consumptive load point driver or control input power  at 25% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most consumptive load point driver or control input power at 50% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most consumptive load point driver or control input power at 100% of BEP </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Most consumptive load point driver or control  input power at 75% of BEP </t>
+  </si>
+  <si>
+    <t>Rated (Least Consumptive) Driver or Control Input Power</t>
+  </si>
+  <si>
+    <t>Most Consumptive Driver or Control Input Power</t>
+  </si>
+  <si>
+    <t>Most Consumptive Pump Energy Index per HI 41.5</t>
+  </si>
+  <si>
+    <t>Most Consumptive Weighted Average Input Power</t>
+  </si>
+  <si>
+    <t>V. External Input Signal  Control and Other Controls</t>
+  </si>
+  <si>
+    <r>
+      <t>Input the most consumptive control method used on the pump.
+Full speed
 Pressure control
-Temperature control</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-External Input signal control only</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
+Temperature control
+External Input signal control only
 External Input signal and other controls</t>
     </r>
     <r>
@@ -408,8 +523,8 @@
   </si>
   <si>
     <r>
-      <t>Input the most consumptive control method used on the pump.
-No speed control
+      <t>Input the Rated (Least Consumptive) control method used on the pump.
+Full speed
 Pressure control
 Temperature control
 External Input signal control only
@@ -439,149 +554,15 @@
     </r>
   </si>
   <si>
-    <t>External Input Signal Only Control</t>
-  </si>
-  <si>
-    <t>External Input Signal and Other Controls</t>
-  </si>
-  <si>
-    <t>Manual Speed Controls</t>
-  </si>
-  <si>
-    <t>CP1: Wet Rotor
-CP2: Dry Rotor Two Piece
-CP3: Dry Rotor Three Piece</t>
-  </si>
-  <si>
-    <t>Control Methods</t>
-  </si>
-  <si>
-    <t>Rated (Least consumptive) HI Energy Rating</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point weigted average input power at maximum rotating speed </t>
-  </si>
-  <si>
-    <t>Rated (Least consumptive) load point weighted average input power at reduced speeds</t>
-  </si>
-  <si>
-    <t>If Pressure speed control is the rated (least consumptive) control method, insert the control curve equation as function of flow rate(x) and head (y). For example y=mx+b or y=ax^2+bx+c, etc.</t>
-  </si>
-  <si>
-    <t>If Pressure speed control is the most consumptive control method, insert the control curve equation as function of flow rate(x) and head(y). For example y=mx+b or y=ax^2+bx+c, etc.</t>
-  </si>
-  <si>
-    <t>Participant/Manufacturer</t>
-  </si>
-  <si>
-    <t>Rated (Least consumptive) Weighted Average Input Power</t>
-  </si>
-  <si>
-    <t>Pressure  Control</t>
-  </si>
-  <si>
-    <t>Tempertature  Control</t>
-  </si>
-  <si>
-    <t>I. No Speed Control</t>
-  </si>
-  <si>
-    <t>II. Pressure  Control</t>
-  </si>
-  <si>
-    <t>III. Temperature Control</t>
-  </si>
-  <si>
-    <t>IV. External Input Signal only  Control</t>
-  </si>
-  <si>
-    <t>VI. Manual Speed Control</t>
-  </si>
-  <si>
-    <t>Input values of maximum and reduced weighted average input power for only control methods V and VI.</t>
-  </si>
-  <si>
-    <t>Input control input power values for only control methods I, II, III, and IV.</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Method I.
-Select Yes if pump uses no speed control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Method II.
-Select Yes if pump uses pressure speed control</t>
-  </si>
-  <si>
-    <t>Method III.
-Select Yes if pump uses temperature speed control</t>
-  </si>
-  <si>
-    <t>Method IV.
-Select Yes if pump uses external input only speed control</t>
-  </si>
-  <si>
-    <t>Method V.
-Select Yes if pump uses external input speed control and other controls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Method VI.
-Select Yes if pump uses manual speed control </t>
-  </si>
-  <si>
-    <t>Fill in for all control methods if applicable</t>
-  </si>
-  <si>
-    <t>Input control input power values for only control methods I, II, III, and IV. Fill in if applicable.</t>
-  </si>
-  <si>
-    <t>Input values of maximum and reduced weighted average input power for only control methods V and VI. Fill in if applicable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point driver or control input power  at 25% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point driver or control input power at 50% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point driver or control  input power at 75% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rated (Least consumptive) load point driver or control input power at 100% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consumptive load point driver or control input power  at 25% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consumptive load point driver or control input power at 50% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consumptive load point driver or control input power at 100% of BEP </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Most consumptive load point driver or control  input power at 75% of BEP </t>
-  </si>
-  <si>
-    <t>Rated (Least Consumptive) Driver or Control Input Power</t>
-  </si>
-  <si>
-    <t>Most Consumptive Driver or Control Input Power</t>
-  </si>
-  <si>
-    <t>Most Consumptive Pump Energy Index per HI 41.5</t>
-  </si>
-  <si>
-    <t>Most Consumptive Weighted Average Input Power</t>
-  </si>
-  <si>
-    <t>V. External Input Signal  Control and Other Controls</t>
+Select Yes if pump uses full speed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1351,6 +1332,39 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1400,39 +1414,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1723,96 +1704,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" customWidth="1"/>
     <col min="14" max="16" width="30" customWidth="1"/>
-    <col min="17" max="17" width="28.140625" customWidth="1"/>
+    <col min="17" max="17" width="28.1640625" customWidth="1"/>
     <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" customWidth="1"/>
-    <col min="20" max="20" width="14.5703125" customWidth="1"/>
-    <col min="21" max="21" width="14.28515625" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" customWidth="1"/>
-    <col min="23" max="23" width="17.28515625" customWidth="1"/>
-    <col min="24" max="25" width="14.28515625" customWidth="1"/>
-    <col min="26" max="26" width="17.28515625" customWidth="1"/>
-    <col min="27" max="29" width="19.140625" customWidth="1"/>
-    <col min="30" max="30" width="12.140625" customWidth="1"/>
-    <col min="31" max="31" width="14.140625" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" customWidth="1"/>
+    <col min="20" max="20" width="14.5" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" customWidth="1"/>
+    <col min="23" max="23" width="17.33203125" customWidth="1"/>
+    <col min="24" max="25" width="14.33203125" customWidth="1"/>
+    <col min="26" max="26" width="17.33203125" customWidth="1"/>
+    <col min="27" max="29" width="19.1640625" customWidth="1"/>
+    <col min="30" max="30" width="12.1640625" customWidth="1"/>
+    <col min="31" max="31" width="14.1640625" customWidth="1"/>
     <col min="32" max="32" width="14" customWidth="1"/>
-    <col min="33" max="34" width="14.7109375" customWidth="1"/>
-    <col min="35" max="35" width="20.28515625" customWidth="1"/>
-    <col min="36" max="36" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="17.85546875" customWidth="1"/>
+    <col min="33" max="34" width="14.6640625" customWidth="1"/>
+    <col min="35" max="35" width="20.33203125" customWidth="1"/>
+    <col min="36" max="36" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="66" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="79"/>
+      <c r="X1" s="80" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y1" s="81"/>
+      <c r="Z1" s="81"/>
+      <c r="AA1" s="81"/>
+      <c r="AB1" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="66" t="s">
-        <v>63</v>
-      </c>
-      <c r="W1" s="68"/>
-      <c r="X1" s="69" t="s">
-        <v>91</v>
-      </c>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="AC1" s="71"/>
-      <c r="AD1" s="63" t="s">
+      <c r="AC1" s="82"/>
+      <c r="AD1" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="64"/>
-      <c r="AG1" s="65"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="75"/>
+      <c r="AG1" s="76"/>
       <c r="AH1" s="26" t="s">
         <v>31</v>
       </c>
@@ -1829,24 +1810,24 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="62"/>
+    <row r="2" spans="1:38" ht="36" x14ac:dyDescent="0.2">
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="73"/>
       <c r="R2" s="39" t="s">
         <v>5</v>
       </c>
@@ -1911,9 +1892,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>0</v>
@@ -1934,22 +1915,22 @@
         <v>3</v>
       </c>
       <c r="H3" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="J3" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="K3" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="J3" s="28" t="s">
+      <c r="L3" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="28" t="s">
         <v>68</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="L3" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="M3" s="28" t="s">
-        <v>70</v>
       </c>
       <c r="N3" s="28" t="s">
         <v>46</v>
@@ -1964,34 +1945,34 @@
         <v>49</v>
       </c>
       <c r="R3" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="U3" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="S3" s="15" t="s">
+      <c r="V3" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="X3" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="T3" s="15" t="s">
+      <c r="Y3" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="U3" s="16" t="s">
+      <c r="Z3" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA3" s="54" t="s">
         <v>85</v>
-      </c>
-      <c r="V3" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="W3" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="X3" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="Y3" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z3" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA3" s="54" t="s">
-        <v>88</v>
       </c>
       <c r="AB3" s="23" t="s">
         <v>32</v>
@@ -2018,16 +1999,16 @@
         <v>39</v>
       </c>
       <c r="AJ3" s="49" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="AK3" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="AL3" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="245.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" ht="245.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>16</v>
@@ -2042,67 +2023,67 @@
         <v>18</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>19</v>
       </c>
       <c r="H4" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="L4" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="M4" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="K4" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="L4" s="30" t="s">
+      <c r="N4" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="P4" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="W4" s="57"/>
+      <c r="X4" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="Y4" s="65"/>
+      <c r="Z4" s="65"/>
+      <c r="AA4" s="63"/>
+      <c r="AB4" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="N4" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="O4" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="P4" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q4" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="R4" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="S4" s="73"/>
-      <c r="T4" s="73"/>
-      <c r="U4" s="74"/>
-      <c r="V4" s="75" t="s">
-        <v>71</v>
-      </c>
-      <c r="W4" s="74"/>
-      <c r="X4" s="81" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="82"/>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="76" t="s">
+      <c r="AC4" s="63"/>
+      <c r="AD4" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="AE4" s="77"/>
-      <c r="AF4" s="77"/>
-      <c r="AG4" s="78"/>
+      <c r="AE4" s="60"/>
+      <c r="AF4" s="60"/>
+      <c r="AG4" s="61"/>
       <c r="AH4" s="52" t="s">
         <v>4</v>
       </c>
@@ -2110,7 +2091,7 @@
         <v>4</v>
       </c>
       <c r="AJ4" s="53" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="AK4" s="21" t="s">
         <v>12</v>
@@ -2121,11 +2102,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="R4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="AD4:AG4"/>
-    <mergeCell ref="AB4:AC4"/>
-    <mergeCell ref="X4:AA4"/>
     <mergeCell ref="A1:G2"/>
     <mergeCell ref="H1:Q2"/>
     <mergeCell ref="AD1:AG1"/>
@@ -2133,25 +2109,30 @@
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="X1:AA1"/>
     <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="AD4:AG4"/>
+    <mergeCell ref="AB4:AC4"/>
+    <mergeCell ref="X4:AA4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Lists!$B$1:$B$3</xm:f>
           </x14:formula1>
           <xm:sqref>F5:F500</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Lists!$C$1:$C$2</xm:f>
           </x14:formula1>
           <xm:sqref>H5:M500</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Lists!$A$1:$A$6</xm:f>
           </x14:formula1>
@@ -2164,20 +2145,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -2188,35 +2169,35 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>